<commit_message>
feat: sops Update 4
</commit_message>
<xml_diff>
--- a/1-Software Development Lifecycle/Forms/FeedBack Survey Form F9.xlsx
+++ b/1-Software Development Lifecycle/Forms/FeedBack Survey Form F9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heba.backar\Downloads\SW 2025 2\SW 2025\SW 2025\1-Software Development Lifecycle\Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QMS\1-Software Development Lifecycle\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C3D0EA-D10D-4433-85AC-2B0148576460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DC8E86-1D51-49B0-8323-BFB0272540E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0FD72531-45CD-44DA-85CA-64CA552C7522}"/>
+    <workbookView xWindow="20370" yWindow="-2595" windowWidth="29040" windowHeight="15840" xr2:uid="{0FD72531-45CD-44DA-85CA-64CA552C7522}"/>
   </bookViews>
   <sheets>
     <sheet name="F-SW-SD-09" sheetId="1" r:id="rId1"/>
@@ -433,21 +433,87 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -465,72 +531,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -904,8 +904,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A12" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,159 +918,159 @@
     <row r="1" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="39"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1078,155 +1078,157 @@
         <v>45</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="33"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="33"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:F8"/>
@@ -1238,37 +1240,35 @@
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:F27"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;16Issue No.:(01)&amp;C&amp;"Arial,Regular"&amp;16F-SW-SD/09&amp;R&amp;"Arial,Regular"&amp;16Rev: 0(0/0/2025)</oddFooter>
+    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;16Issue No.:(01)&amp;C&amp;"Arial,Regular"&amp;16F-SW-SD/09&amp;R&amp;"Arial,Regular"&amp;16Rev:0(01/10/2025)</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select your department from the drop list" xr:uid="{1B1EE51F-BF2A-4F31-B845-9092864A5B6D}">
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$11</xm:f>

</xml_diff>